<commit_message>
plantilla lista de asistencia - detalle
</commit_message>
<xml_diff>
--- a/XLSX/plantillaListaAsistencia.xlsx
+++ b/XLSX/plantillaListaAsistencia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Residencia\Pruebas\pruebaLogin\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Final\actdoc\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5FEE15-4E66-4864-B65B-D8EBC69B3A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B67A4B-ED69-4670-81DE-ACB850FC39F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="0" windowWidth="20280" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato" sheetId="1" r:id="rId1"/>
@@ -835,7 +835,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -876,11 +876,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1007,6 +1002,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1505,8 +1503,8 @@
   </sheetPr>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:H42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1523,80 +1521,80 @@
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:15" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-      <c r="B2" s="69" t="s">
+      <c r="A2" s="79"/>
+      <c r="B2" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="89" t="s">
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="91"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="89"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
-      <c r="B3" s="72" t="s">
+      <c r="A3" s="80"/>
+      <c r="B3" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="89" t="s">
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="91"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="89"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="82"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="89" t="s">
+      <c r="A4" s="80"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="91"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="89"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="83"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="92" t="s">
+      <c r="A5" s="81"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="91"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="89"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1608,32 +1606,32 @@
       <c r="D6"/>
     </row>
     <row r="8" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="85" t="s">
+      <c r="C8" s="85"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
     </row>
     <row r="10" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
@@ -1653,10 +1651,10 @@
       <c r="G11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
     </row>
     <row r="13" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1664,33 +1662,33 @@
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="94" t="s">
+      <c r="E13" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="94"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="20"/>
     </row>
     <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="2" t="s">
         <v>59</v>
       </c>
@@ -1699,40 +1697,40 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="38"/>
+      <c r="B17" s="35"/>
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="84" t="s">
+      <c r="D19" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="E19" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84" t="s">
+      <c r="F19" s="82"/>
+      <c r="G19" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
     </row>
     <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="84"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="84"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="16"/>
@@ -1740,10 +1738,10 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="84"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="10" t="s">
         <v>19</v>
       </c>
@@ -1773,8 +1771,8 @@
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
@@ -1788,8 +1786,8 @@
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
@@ -1803,8 +1801,8 @@
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -1818,8 +1816,8 @@
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
@@ -1833,8 +1831,8 @@
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
@@ -1848,13 +1846,13 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="19"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
     </row>
     <row r="28" spans="1:11" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
@@ -1863,8 +1861,8 @@
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
@@ -1878,8 +1876,8 @@
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
@@ -1893,8 +1891,8 @@
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -1908,8 +1906,8 @@
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
@@ -1923,8 +1921,8 @@
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
@@ -1938,8 +1936,8 @@
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -1953,8 +1951,8 @@
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
@@ -1968,8 +1966,8 @@
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
@@ -1983,8 +1981,8 @@
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -1998,8 +1996,8 @@
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
@@ -2013,8 +2011,8 @@
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
@@ -2027,26 +2025,26 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="68"/>
-      <c r="B42" s="68"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="67" t="s">
+      <c r="A43" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="67"/>
-      <c r="D43" s="93" t="s">
+      <c r="B43" s="65"/>
+      <c r="D43" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
@@ -2113,330 +2111,330 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="24" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="25" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="24" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="21" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="97" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="93" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="94"/>
     </row>
     <row r="3" spans="1:11" ht="95.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="37">
         <v>43269</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="38">
         <v>43280</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="27">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="53" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="44">
         <v>43276</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="44">
         <v>43280</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="43">
         <v>30</v>
       </c>
-      <c r="J4" s="44"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="44">
         <v>43276</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="44">
         <v>43280</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="43">
         <v>30</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="59"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="56"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="48" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="44">
         <v>43276</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="44">
         <v>43280</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="46">
         <v>30</v>
       </c>
-      <c r="I6" s="59"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="51" t="s">
+      <c r="B7" s="42"/>
+      <c r="C7" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="44">
         <v>43276</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="44">
         <v>43280</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="46">
         <v>30</v>
       </c>
-      <c r="I7" s="59"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="59"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="56"/>
     </row>
     <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="56" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="44">
         <v>43276</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="44">
         <v>43280</v>
       </c>
-      <c r="F8" s="49">
+      <c r="F8" s="46">
         <v>30</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="59"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="56"/>
     </row>
     <row r="9" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="65" t="s">
+      <c r="B9" s="60"/>
+      <c r="C9" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="61">
         <v>43269</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="26">
         <v>43273</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="32">
         <v>30</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="59"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="56"/>
     </row>
     <row r="10" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="50" t="s">
+      <c r="B10" s="58"/>
+      <c r="C10" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="61">
         <v>43269</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="26">
         <v>43273</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="32">
         <v>30</v>
       </c>
-      <c r="I10" s="59"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="59"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="56"/>
     </row>
     <row r="11" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="50" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="61">
         <v>43269</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="26">
         <v>43273</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="32">
         <v>30</v>
       </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
     </row>
     <row r="12" spans="1:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="50" t="s">
+      <c r="B12" s="58"/>
+      <c r="C12" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="61">
         <v>43269</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="26">
         <v>43273</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="32">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="35"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="35"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="33"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="33"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="33"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="31"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="33"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="33"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="31"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="33"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="33"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="33"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="31"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="35"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>